<commit_message>
Finished naked planet spreadsheet
</commit_message>
<xml_diff>
--- a/naked-planet/spreadsheet.xlsx
+++ b/naked-planet/spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MrMil\dev\global-warming-modelling\naked-planet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127C0C19-C990-464C-BF68-18E205F11C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F589E6E3-2C68-48C9-AB2D-3F0EBA873868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>L (W/m2)</t>
   </si>
@@ -59,25 +59,10 @@
     <t>Time step</t>
   </si>
   <si>
-    <t>d Heat Content/dt</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
     <t>Initial Temperature</t>
   </si>
   <si>
     <t>Heat Capacity (J/m2 K)</t>
-  </si>
-  <si>
-    <t>Outflux</t>
-  </si>
-  <si>
-    <t>Influx (W)</t>
-  </si>
-  <si>
-    <t>Heat Content (J)</t>
   </si>
   <si>
     <t>Time (Y)</t>
@@ -95,10 +80,31 @@
     <t>Water Surface (m2)</t>
   </si>
   <si>
-    <t>Water Specific Heat Capacity (J/g)</t>
+    <t>Water Mass (kg)</t>
   </si>
   <si>
-    <t>Water Mass (kg)</t>
+    <t>Water Specific Heat Capacity (J/kg K)</t>
+  </si>
+  <si>
+    <t>Heat Content (J/m2)</t>
+  </si>
+  <si>
+    <t>Temperature (K)</t>
+  </si>
+  <si>
+    <t>Outflux (W/m2)</t>
+  </si>
+  <si>
+    <t>Influx (W/m2)</t>
+  </si>
+  <si>
+    <t>d Heat Content/dt (W/m2)</t>
+  </si>
+  <si>
+    <t>dHeatContent/dt (J/m2)</t>
+  </si>
+  <si>
+    <t>Seconds in Year</t>
   </si>
 </sst>
 </file>
@@ -134,9 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,204 +231,144 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$38</c:f>
+              <c:f>Sheet1!$C$8:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>700</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="17">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>900</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="19">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2100</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2300</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2600</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2700</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2800</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2900</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$8:$E$38</c:f>
+              <c:f>Sheet1!$E$8:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.00000086940199</c:v>
+                  <c:v>213.70873014832645</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200.00000173880395</c:v>
+                  <c:v>224.82235106617364</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200.00000260820588</c:v>
+                  <c:v>233.43140114436179</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>200.00000347760781</c:v>
+                  <c:v>239.82723249429046</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>200.00000434700974</c:v>
+                  <c:v>244.41226706258308</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>200.00000521641164</c:v>
+                  <c:v>247.60683700050046</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>200.00000608581354</c:v>
+                  <c:v>249.78521822445362</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>200.00000695521544</c:v>
+                  <c:v>251.24772558136772</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>200.00000782461734</c:v>
+                  <c:v>252.21898768320796</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>200.00000869401921</c:v>
+                  <c:v>252.85923445442012</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200.00000956342109</c:v>
+                  <c:v>253.27917752848208</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200.00001043282293</c:v>
+                  <c:v>253.5537098982692</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>200.00001130222478</c:v>
+                  <c:v>253.73279009700087</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>200.00001217162662</c:v>
+                  <c:v>253.84943857600226</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>200.00001304102844</c:v>
+                  <c:v>253.92534939402796</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>200.00001391043025</c:v>
+                  <c:v>253.97471936110136</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>200.00001477983207</c:v>
+                  <c:v>254.00681522862868</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>200.00001564923389</c:v>
+                  <c:v>254.0276756412969</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>200.00001651863568</c:v>
+                  <c:v>254.04123138984156</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200.00001738803746</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>200.00001825743925</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>200.00001912684101</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>200.00001999624277</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>200.00002086564453</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>200.00002173504626</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>200.00002260444799</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>200.00002347384972</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>200.00002434325143</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>200.0000252126531</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>200.0000260820548</c:v>
+                  <c:v>254.05003937443249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1495,15 +1442,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I38"/>
+  <dimension ref="B2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -1520,15 +1470,18 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>1350</v>
@@ -1549,34 +1502,37 @@
         <f>$C$3*(1-$D$3)/4</f>
         <v>236.24999999999997</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K3" s="2">
+        <v>31536000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
       <c r="I4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4000</v>
       </c>
@@ -1587,46 +1543,49 @@
         <f>4/3*PI()*(($B$5+$C$5)^3 - $C$5^3)</f>
         <v>2.0415391212767142E+18</v>
       </c>
-      <c r="E5">
-        <v>997</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="E5" s="1">
         <f>4*PI()*($B$5+$C$5)^2</f>
         <v>510705155749190.75</v>
       </c>
+      <c r="F5">
+        <v>997</v>
+      </c>
       <c r="G5" s="1">
-        <f>$D$5*$E$5</f>
+        <f>$D$5*$F$5</f>
         <v>2.0354145039128841E+21</v>
       </c>
       <c r="H5">
-        <v>4.2</v>
+        <v>4200</v>
       </c>
       <c r="I5" s="1">
-        <f>1000*$G$5*$H$5/$F$5</f>
+        <f>$G$5*$H$5/$E$5</f>
         <v>16739092645.135607</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0</v>
       </c>
@@ -1650,759 +1609,664 @@
         <f>$H$3 - F8</f>
         <v>145.52999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
+        <f>G8*$K$3</f>
+        <v>4589434079.999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C38" si="0">$B$3*B9</f>
-        <v>100</v>
+        <f>$B$3*B9</f>
+        <v>50</v>
       </c>
       <c r="D9" s="1">
-        <f>D8+G8*$B$3</f>
-        <v>3347818543580.1216</v>
+        <f>D8+H8*$B$3</f>
+        <v>3577290233027.1216</v>
       </c>
       <c r="E9" s="1">
         <f>D9/$I$5</f>
-        <v>200.00000086940199</v>
+        <v>213.70873014832645</v>
       </c>
       <c r="F9" s="1">
         <f>$E$3*$F$3*(E9^4)</f>
-        <v>90.720001577442986</v>
+        <v>118.2693238414758</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" ref="G9:G38" si="1">$H$3 - F9</f>
-        <v>145.52999842255699</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <f>$H$3 - F9</f>
+        <v>117.98067615852418</v>
+      </c>
+      <c r="H9" s="1">
+        <f>G9*$K$3</f>
+        <v>3720638603.3352184</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>200</v>
+        <f>$B$3*B10</f>
+        <v>100</v>
       </c>
       <c r="D10" s="1">
-        <f>D9+G9*$B$3</f>
-        <v>3347818558133.1216</v>
+        <f>D9+H9*$B$3</f>
+        <v>3763322163193.8823</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" ref="E10:E38" si="2">D10/$I$5</f>
-        <v>200.00000173880395</v>
+        <f>D10/$I$5</f>
+        <v>224.82235106617364</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" ref="F9:F38" si="3">$E$3*$F$3*(E10^4)</f>
-        <v>90.720003154885902</v>
+        <f>$E$3*$F$3*(E10^4)</f>
+        <v>144.85750453741534</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52999684511406</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <f>$H$3 - F10</f>
+        <v>91.392495462584634</v>
+      </c>
+      <c r="H10" s="1">
+        <f>G10*$K$3</f>
+        <v>2882153736.9080691</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f>$B$3*B11</f>
+        <v>150</v>
       </c>
       <c r="D11" s="1">
-        <f>D10+G10*$B$3</f>
-        <v>3347818572686.1211</v>
+        <f>D10+H10*$B$3</f>
+        <v>3907429850039.2856</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00000260820588</v>
+        <f>D11/$I$5</f>
+        <v>233.43140114436179</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720004732328817</v>
+        <f>$E$3*$F$3*(E11^4)</f>
+        <v>168.35273115860011</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52999526767115</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+        <f>$H$3 - F11</f>
+        <v>67.897268841399864</v>
+      </c>
+      <c r="H11" s="1">
+        <f>G11*$K$3</f>
+        <v>2141208270.1823862</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>400</v>
+        <f>$B$3*B12</f>
+        <v>200</v>
       </c>
       <c r="D12" s="1">
-        <f>D11+G11*$B$3</f>
-        <v>3347818587239.1206</v>
+        <f>D11+H11*$B$3</f>
+        <v>4014490263548.4048</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00000347760781</v>
+        <f t="shared" ref="E12:E38" si="0">D12/$I$5</f>
+        <v>239.82723249429046</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720006309771776</v>
+        <f>$E$3*$F$3*(E12^4)</f>
+        <v>187.57590156024909</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>145.5299936902282</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <f>$H$3 - F12</f>
+        <v>48.674098439750878</v>
+      </c>
+      <c r="H12" s="1">
+        <f>G12*$K$3</f>
+        <v>1534986368.3959837</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13">
+        <f>$B$3*B13</f>
+        <v>250</v>
+      </c>
+      <c r="D13" s="1">
+        <f>D12+H12*$B$3</f>
+        <v>4091239581968.2041</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="D13" s="1">
-        <f>D12+G12*$B$3</f>
-        <v>3347818601792.1201</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00000434700974</v>
+        <v>244.41226706258308</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="3"/>
-        <v>90.72000788721472</v>
+        <f>$E$3*$F$3*(E13^4)</f>
+        <v>202.33688346514188</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52999211278524</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <f>$H$3 - F13</f>
+        <v>33.913116534858091</v>
+      </c>
+      <c r="H13" s="1">
+        <f>G13*$K$3</f>
+        <v>1069484043.0432848</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14">
+        <f>$B$3*B14</f>
+        <v>300</v>
+      </c>
+      <c r="D14" s="1">
+        <f>D13+H13*$B$3</f>
+        <v>4144713784120.3682</v>
+      </c>
+      <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-      <c r="D14" s="1">
-        <f>D13+G13*$B$3</f>
-        <v>3347818616345.1191</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00000521641164</v>
+        <v>247.60683700050046</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720009464657636</v>
+        <f>$E$3*$F$3*(E14^4)</f>
+        <v>213.12460354884851</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52999053534234</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+        <f>$H$3 - F14</f>
+        <v>23.12539645115146</v>
+      </c>
+      <c r="H14" s="1">
+        <f>G14*$K$3</f>
+        <v>729282502.4835124</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>7</v>
       </c>
       <c r="C15">
+        <f>$B$3*B15</f>
+        <v>350</v>
+      </c>
+      <c r="D15" s="1">
+        <f>D14+H14*$B$3</f>
+        <v>4181177909244.5439</v>
+      </c>
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>700</v>
-      </c>
-      <c r="D15" s="1">
-        <f>D14+G14*$B$3</f>
-        <v>3347818630898.1182</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00000608581354</v>
+        <v>249.78521822445362</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720011042100595</v>
+        <f>$E$3*$F$3*(E15^4)</f>
+        <v>220.72422238611256</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52998895789938</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+        <f>$H$3 - F15</f>
+        <v>15.525777613887414</v>
+      </c>
+      <c r="H15" s="1">
+        <f>G15*$K$3</f>
+        <v>489620922.83155346</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16">
+        <f>$B$3*B16</f>
+        <v>400</v>
+      </c>
+      <c r="D16" s="1">
+        <f>D15+H15*$B$3</f>
+        <v>4205658955386.1216</v>
+      </c>
+      <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="D16" s="1">
-        <f>D15+G15*$B$3</f>
-        <v>3347818645451.1172</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00000695521544</v>
+        <v>251.24772558136772</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720012619543539</v>
+        <f>$E$3*$F$3*(E16^4)</f>
+        <v>225.93921467185879</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52998738045642</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F16</f>
+        <v>10.310785328141179</v>
+      </c>
+      <c r="H16" s="1">
+        <f>G16*$K$3</f>
+        <v>325160926.10826021</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>9</v>
       </c>
       <c r="C17">
+        <f>$B$3*B17</f>
+        <v>450</v>
+      </c>
+      <c r="D17" s="1">
+        <f>D16+H16*$B$3</f>
+        <v>4221917001691.5347</v>
+      </c>
+      <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="D17" s="1">
-        <f>D16+G16*$B$3</f>
-        <v>3347818660004.1157</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00000782461734</v>
+        <v>252.21898768320796</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="3"/>
-        <v>90.72001419698654</v>
+        <f>$E$3*$F$3*(E17^4)</f>
+        <v>229.45322804473022</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52998580301343</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F17</f>
+        <v>6.7967719552697474</v>
+      </c>
+      <c r="H17" s="1">
+        <f>G17*$K$3</f>
+        <v>214343000.38138676</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>10</v>
       </c>
       <c r="C18">
+        <f>$B$3*B18</f>
+        <v>500</v>
+      </c>
+      <c r="D18" s="1">
+        <f>D17+H17*$B$3</f>
+        <v>4232634151710.604</v>
+      </c>
+      <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D18" s="1">
-        <f>D17+G17*$B$3</f>
-        <v>3347818674557.1143</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00000869401921</v>
+        <v>252.85923445442012</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="3"/>
-        <v>90.72001577442947</v>
+        <f>$E$3*$F$3*(E18^4)</f>
+        <v>231.79194189345102</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="1"/>
-        <v>145.5299842255705</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F18</f>
+        <v>4.4580581065489469</v>
+      </c>
+      <c r="H18" s="1">
+        <f>G18*$K$3</f>
+        <v>140589320.4481276</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>11</v>
       </c>
       <c r="C19">
+        <f>$B$3*B19</f>
+        <v>550</v>
+      </c>
+      <c r="D19" s="1">
+        <f>D18+H18*$B$3</f>
+        <v>4239663617733.0103</v>
+      </c>
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>1100</v>
-      </c>
-      <c r="D19" s="1">
-        <f>D18+G18*$B$3</f>
-        <v>3347818689110.1128</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00000956342109</v>
+        <v>253.27917752848208</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720017351872471</v>
+        <f>$E$3*$F$3*(E19^4)</f>
+        <v>233.33560199647687</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52998264812749</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F19</f>
+        <v>2.9143980035231039</v>
+      </c>
+      <c r="H19" s="1">
+        <f>G19*$K$3</f>
+        <v>91908455.439104602</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>12</v>
       </c>
       <c r="C20">
+        <f>$B$3*B20</f>
+        <v>600</v>
+      </c>
+      <c r="D20" s="1">
+        <f>D19+H19*$B$3</f>
+        <v>4244259040504.9653</v>
+      </c>
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="D20" s="1">
-        <f>D19+G19*$B$3</f>
-        <v>3347818703663.1108</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001043282293</v>
+        <v>253.5537098982692</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720018929315401</v>
+        <f>$E$3*$F$3*(E20^4)</f>
+        <v>234.34890915938712</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52998107068458</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F20</f>
+        <v>1.9010908406128522</v>
+      </c>
+      <c r="H20" s="1">
+        <f>G20*$K$3</f>
+        <v>59952800.749566905</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>13</v>
       </c>
       <c r="C21">
+        <f>$B$3*B21</f>
+        <v>650</v>
+      </c>
+      <c r="D21" s="1">
+        <f>D20+H20*$B$3</f>
+        <v>4247256680542.4438</v>
+      </c>
+      <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>1300</v>
-      </c>
-      <c r="D21" s="1">
-        <f>D20+G20*$B$3</f>
-        <v>3347818718216.1089</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001130222478</v>
+        <v>253.73279009700087</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720020506758374</v>
+        <f>$E$3*$F$3*(E21^4)</f>
+        <v>235.01167573762137</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="1"/>
-        <v>145.5299794932416</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F21</f>
+        <v>1.2383242623785975</v>
+      </c>
+      <c r="H21" s="1">
+        <f>G21*$K$3</f>
+        <v>39051793.93837145</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>14</v>
       </c>
       <c r="C22">
+        <f>$B$3*B22</f>
+        <v>700</v>
+      </c>
+      <c r="D22" s="1">
+        <f>D21+H21*$B$3</f>
+        <v>4249209270239.3623</v>
+      </c>
+      <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>1400</v>
-      </c>
-      <c r="D22" s="1">
-        <f>D21+G21*$B$3</f>
-        <v>3347818732769.1069</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001217162662</v>
+        <v>253.84943857600226</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720022084201347</v>
+        <f>$E$3*$F$3*(E22^4)</f>
+        <v>235.4441411620368</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52997791579861</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F22</f>
+        <v>0.80585883796317148</v>
+      </c>
+      <c r="H22" s="1">
+        <f>G22*$K$3</f>
+        <v>25413564.314006574</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>15</v>
       </c>
       <c r="C23">
+        <f>$B$3*B23</f>
+        <v>750</v>
+      </c>
+      <c r="D23" s="1">
+        <f>D22+H22*$B$3</f>
+        <v>4250479948455.0625</v>
+      </c>
+      <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="D23" s="1">
-        <f>D22+G22*$B$3</f>
-        <v>3347818747322.1045</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001304102844</v>
+        <v>253.92534939402796</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720023661644319</v>
+        <f>$E$3*$F$3*(E23^4)</f>
+        <v>235.72589519740669</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52997633835565</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F23</f>
+        <v>0.52410480259328551</v>
+      </c>
+      <c r="H23" s="1">
+        <f>G23*$K$3</f>
+        <v>16528169.054581853</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>16</v>
       </c>
       <c r="C24">
+        <f>$B$3*B24</f>
+        <v>800</v>
+      </c>
+      <c r="D24" s="1">
+        <f>D23+H23*$B$3</f>
+        <v>4251306356907.7915</v>
+      </c>
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>1600</v>
-      </c>
-      <c r="D24" s="1">
-        <f>D23+G23*$B$3</f>
-        <v>3347818761875.1021</v>
-      </c>
-      <c r="E24" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001391043025</v>
+        <v>253.97471936110136</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720025239087278</v>
+        <f>$E$3*$F$3*(E24^4)</f>
+        <v>235.90927467017627</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52997476091269</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F24</f>
+        <v>0.34072532982369808</v>
+      </c>
+      <c r="H24" s="1">
+        <f>G24*$K$3</f>
+        <v>10745114.001320142</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>17</v>
       </c>
       <c r="C25">
+        <f>$B$3*B25</f>
+        <v>850</v>
+      </c>
+      <c r="D25" s="1">
+        <f>D24+H24*$B$3</f>
+        <v>4251843612607.8574</v>
+      </c>
+      <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>1700</v>
-      </c>
-      <c r="D25" s="1">
-        <f>D24+G24*$B$3</f>
-        <v>3347818776428.0996</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001477983207</v>
+        <v>254.00681522862868</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720026816530279</v>
+        <f>$E$3*$F$3*(E25^4)</f>
+        <v>236.02854871875368</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52997318346968</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F25</f>
+        <v>0.22145128124628854</v>
+      </c>
+      <c r="H25" s="1">
+        <f>G25*$K$3</f>
+        <v>6983687.6053829556</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>18</v>
       </c>
       <c r="C26">
+        <f>$B$3*B26</f>
+        <v>900</v>
+      </c>
+      <c r="D26" s="1">
+        <f>D25+H25*$B$3</f>
+        <v>4252192796988.1265</v>
+      </c>
+      <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>1800</v>
-      </c>
-      <c r="D26" s="1">
-        <f>D25+G25*$B$3</f>
-        <v>3347818790981.0972</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001564923389</v>
+        <v>254.0276756412969</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720028393973294</v>
+        <f>$E$3*$F$3*(E26^4)</f>
+        <v>236.10609403173308</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52997160602666</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F26</f>
+        <v>0.14390596826689261</v>
+      </c>
+      <c r="H26" s="1">
+        <f>G26*$K$3</f>
+        <v>4538218.6152647259</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>19</v>
       </c>
       <c r="C27">
+        <f>$B$3*B27</f>
+        <v>950</v>
+      </c>
+      <c r="D27" s="1">
+        <f>D26+H26*$B$3</f>
+        <v>4252419707918.8896</v>
+      </c>
+      <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>1900</v>
-      </c>
-      <c r="D27" s="1">
-        <f>D26+G26*$B$3</f>
-        <v>3347818805534.0942</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001651863568</v>
+        <v>254.04123138984156</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720029971416295</v>
+        <f>$E$3*$F$3*(E27^4)</f>
+        <v>236.15649564302083</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52997002858368</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+        <f>$H$3 - F27</f>
+        <v>9.3504356979138947E-2</v>
+      </c>
+      <c r="H27" s="1">
+        <f>G27*$K$3</f>
+        <v>2948753.401694126</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>20</v>
       </c>
       <c r="C28">
+        <f>$B$3*B28</f>
+        <v>1000</v>
+      </c>
+      <c r="D28" s="1">
+        <f>D27+H27*$B$3</f>
+        <v>4252567145588.9741</v>
+      </c>
+      <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="D28" s="1">
-        <f>D27+G27*$B$3</f>
-        <v>3347818820087.0913</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001738803746</v>
+        <v>254.05003937443249</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720031548859268</v>
+        <f>$E$3*$F$3*(E28^4)</f>
+        <v>236.18924892395972</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52996845114069</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>21</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>2100</v>
-      </c>
-      <c r="D29" s="1">
-        <f>D28+G28*$B$3</f>
-        <v>3347818834640.0884</v>
-      </c>
-      <c r="E29" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001825743925</v>
-      </c>
-      <c r="F29" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720033126302297</v>
-      </c>
-      <c r="G29" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52996687369767</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>22</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>2200</v>
-      </c>
-      <c r="D30" s="1">
-        <f>D29+G29*$B$3</f>
-        <v>3347818849193.085</v>
-      </c>
-      <c r="E30" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001912684101</v>
-      </c>
-      <c r="F30" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720034703745313</v>
-      </c>
-      <c r="G30" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52996529625466</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>23</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>2300</v>
-      </c>
-      <c r="D31" s="1">
-        <f>D30+G30*$B$3</f>
-        <v>3347818863746.0815</v>
-      </c>
-      <c r="E31" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00001999624277</v>
-      </c>
-      <c r="F31" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720036281188328</v>
-      </c>
-      <c r="G31" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52996371881164</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>24</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>2400</v>
-      </c>
-      <c r="D32" s="1">
-        <f>D31+G31*$B$3</f>
-        <v>3347818878299.0781</v>
-      </c>
-      <c r="E32" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00002086564453</v>
-      </c>
-      <c r="F32" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720037858631372</v>
-      </c>
-      <c r="G32" s="1">
-        <f t="shared" si="1"/>
-        <v>145.5299621413686</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>25</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>2500</v>
-      </c>
-      <c r="D33" s="1">
-        <f>D32+G32*$B$3</f>
-        <v>3347818892852.0742</v>
-      </c>
-      <c r="E33" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00002173504626</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720039436074373</v>
-      </c>
-      <c r="G33" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52996056392561</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>26</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="0"/>
-        <v>2600</v>
-      </c>
-      <c r="D34" s="1">
-        <f>D33+G33*$B$3</f>
-        <v>3347818907405.0703</v>
-      </c>
-      <c r="E34" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00002260444799</v>
-      </c>
-      <c r="F34" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720041013517402</v>
-      </c>
-      <c r="G34" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52995898648257</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <v>27</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>2700</v>
-      </c>
-      <c r="D35" s="1">
-        <f>D34+G34*$B$3</f>
-        <v>3347818921958.0664</v>
-      </c>
-      <c r="E35" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00002347384972</v>
-      </c>
-      <c r="F35" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720042590960446</v>
-      </c>
-      <c r="G35" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52995740903953</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <v>28</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="0"/>
-        <v>2800</v>
-      </c>
-      <c r="D36" s="1">
-        <f>D35+G35*$B$3</f>
-        <v>3347818936511.062</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" si="2"/>
-        <v>200.00002434325143</v>
-      </c>
-      <c r="F36" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720044168403433</v>
-      </c>
-      <c r="G36" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52995583159654</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>29</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="0"/>
-        <v>2900</v>
-      </c>
-      <c r="D37" s="1">
-        <f>D36+G36*$B$3</f>
-        <v>3347818951064.0576</v>
-      </c>
-      <c r="E37" s="1">
-        <f t="shared" si="2"/>
-        <v>200.0000252126531</v>
-      </c>
-      <c r="F37" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720045745846434</v>
-      </c>
-      <c r="G37" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52995425415355</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>30</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-      <c r="D38" s="1">
-        <f>D37+G37*$B$3</f>
-        <v>3347818965617.0532</v>
-      </c>
-      <c r="E38" s="1">
-        <f t="shared" si="2"/>
-        <v>200.0000260820548</v>
-      </c>
-      <c r="F38" s="1">
-        <f t="shared" si="3"/>
-        <v>90.720047323289492</v>
-      </c>
-      <c r="G38" s="1">
-        <f t="shared" si="1"/>
-        <v>145.52995267671048</v>
-      </c>
+        <f>$H$3 - F28</f>
+        <v>6.0751076040247654E-2</v>
+      </c>
+      <c r="H28" s="1">
+        <f>G28*$K$3</f>
+        <v>1915845.93400525</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>